<commit_message>
git commit -m ""
</commit_message>
<xml_diff>
--- a/modelo_planilha.xlsx
+++ b/modelo_planilha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://samarces-my.sharepoint.com/personal/joabe_alves_samarces_onmicrosoft_com/Documents/Projeto_Auto_Experts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2B59D2BFD300D5B91921AD53583088B35299F25E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{806F48EE-93FA-4112-88A2-CB0AE223A102}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_2B59D2BFD350DD434459A813493088B35299F0F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86FAB329-BD61-4A22-AEB1-84AA438FBA11}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="3060" windowWidth="12690" windowHeight="9165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Código Produto</t>
   </si>
@@ -37,6 +37,12 @@
     <t>Peso</t>
   </si>
   <si>
+    <t>Código de barras (EAN)</t>
+  </si>
+  <si>
+    <t>NCM</t>
+  </si>
+  <si>
     <t>C-5682</t>
   </si>
   <si>
@@ -52,6 +58,12 @@
     <t>2,996</t>
   </si>
   <si>
+    <t>7893049568296</t>
+  </si>
+  <si>
+    <t>87083090</t>
+  </si>
+  <si>
     <t>HG 41123</t>
   </si>
   <si>
@@ -65,6 +77,12 @@
   </si>
   <si>
     <t>3,200</t>
+  </si>
+  <si>
+    <t>7890903099835</t>
+  </si>
+  <si>
+    <t>8708.80.00</t>
   </si>
 </sst>
 </file>
@@ -427,19 +445,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,39 +472,57 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
git -m commit 'Melhora na função de requisição'
</commit_message>
<xml_diff>
--- a/modelo_planilha.xlsx
+++ b/modelo_planilha.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://samarces-my.sharepoint.com/personal/joabe_alves_samarces_onmicrosoft_com/Documents/Projeto_Auto_Experts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_2B59D2BFD350DD434459A813493088B35299F0F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86FAB329-BD61-4A22-AEB1-84AA438FBA11}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59D2BFD3A05A48B6C30F73403088B352998CF8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD0C4BD2-06A2-4B9F-A46E-EB39702306A3}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="3060" windowWidth="12690" windowHeight="9165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Código Produto</t>
   </si>
@@ -43,46 +43,19 @@
     <t>NCM</t>
   </si>
   <si>
-    <t>C-5682</t>
-  </si>
-  <si>
-    <t>SERVO FREIO CONTROIL - C-5682</t>
-  </si>
-  <si>
-    <t>CONTROIL</t>
-  </si>
-  <si>
-    <t>PEUGEOT 2008 1.0 12V/1.6 16V 2015-2024 208 1.2 12V/1.5 8V/1.6 16V 2013-2024 CITROEN C3 1.2 12V/1.5 8V/1.6 16V 2012-2021 AIRCROSS 1.5 8V/1.6 16V 2010-2021</t>
-  </si>
-  <si>
-    <t>2,996</t>
-  </si>
-  <si>
-    <t>7893049568296</t>
-  </si>
-  <si>
-    <t>87083090</t>
-  </si>
-  <si>
-    <t>HG 41123</t>
-  </si>
-  <si>
-    <t>AMORTECEDOR DE SUSPENSÃO DIANTEIRO ESQUERDO NAKATA - HG 41123</t>
-  </si>
-  <si>
-    <t>NAKATA</t>
-  </si>
-  <si>
-    <t>HYUNDAI HB20 X 1.0 12V/1.6 16V 2012-2019</t>
-  </si>
-  <si>
-    <t>3,200</t>
-  </si>
-  <si>
-    <t>7890903099835</t>
-  </si>
-  <si>
-    <t>8708.80.00</t>
+    <t>C-2184</t>
+  </si>
+  <si>
+    <t>AC 30937</t>
+  </si>
+  <si>
+    <t>HG 30784</t>
+  </si>
+  <si>
+    <t>BD3442</t>
+  </si>
+  <si>
+    <t>BD4190</t>
   </si>
 </sst>
 </file>
@@ -445,16 +418,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -483,46 +451,25 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>